<commit_message>
Changes in DataProvider for POST User added
</commit_message>
<xml_diff>
--- a/src/test/java/restAPI/dataProviderData/ExcelData.xlsx
+++ b/src/test/java/restAPI/dataProviderData/ExcelData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>email</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>12345@mail.ru</t>
-  </si>
-  <si>
     <t>can't be blank</t>
   </si>
   <si>
@@ -73,6 +70,27 @@
   </si>
   <si>
     <t>can be Male or Female</t>
+  </si>
+  <si>
+    <t>User2@ukr.net</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>can be Active or Inactive</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>123456@mail.ru</t>
   </si>
 </sst>
 </file>
@@ -117,10 +135,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -402,17 +421,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -443,8 +462,8 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -452,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -460,8 +479,8 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -469,7 +488,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -477,8 +496,8 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -491,17 +510,139 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New negative cases for POST User added
</commit_message>
<xml_diff>
--- a/src/test/java/restAPI/dataProviderData/ExcelData.xlsx
+++ b/src/test/java/restAPI/dataProviderData/ExcelData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
   <si>
     <t>email</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Admin@ukr.net</t>
   </si>
   <si>
-    <t>User@ukr.net</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -66,15 +63,9 @@
     <t>can't be blank</t>
   </si>
   <si>
-    <t>has already been taken</t>
-  </si>
-  <si>
     <t>can be Male or Female</t>
   </si>
   <si>
-    <t>User2@ukr.net</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -90,7 +81,19 @@
     <t>""</t>
   </si>
   <si>
-    <t>123456@mail.ru</t>
+    <t>!@#$%^</t>
+  </si>
+  <si>
+    <t>in case if uses null as cell value, set cell format as text</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>is invalid</t>
+  </si>
+  <si>
+    <t>Admin4@ukr.net</t>
   </si>
 </sst>
 </file>
@@ -421,37 +424,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -460,189 +463,391 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B4" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId3"/>
+    <hyperlink ref="C14" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5" display="Admin3@ukr.net"/>
+    <hyperlink ref="B10" r:id="rId6" display="Admin2@ukr.net"/>
+    <hyperlink ref="B11" r:id="rId7" display="Admin2@ukr.net"/>
+    <hyperlink ref="B12" r:id="rId8" display="Admin2@ukr.net"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B15" r:id="rId10" display="Admin2@ukr.net"/>
+    <hyperlink ref="B16" r:id="rId11" display="Admin2@ukr.net"/>
+    <hyperlink ref="B17" r:id="rId12" display="Admin2@ukr.net"/>
+    <hyperlink ref="B18" r:id="rId13" display="Admin2@ukr.net"/>
+    <hyperlink ref="B19" r:id="rId14" display="Admin2@ukr.net"/>
+    <hyperlink ref="B20" r:id="rId15" display="Admin2@ukr.net"/>
+    <hyperlink ref="B21" r:id="rId16" display="Admin2@ukr.net"/>
+    <hyperlink ref="B7" r:id="rId17" display="Admin2@ukr.net"/>
+    <hyperlink ref="B5" r:id="rId18" display="Admin2@ukr.net"/>
+    <hyperlink ref="B3" r:id="rId19" display="Admin2@ukr.net"/>
+    <hyperlink ref="B22" r:id="rId20" display="!@#$%^"/>
+    <hyperlink ref="B23" r:id="rId21" display="!@#$%^"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complex models and tests fix
</commit_message>
<xml_diff>
--- a/src/test/java/restAPI/dataProviderData/ExcelData.xlsx
+++ b/src/test/java/restAPI/dataProviderData/ExcelData.xlsx
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Admin@ukr.net</t>
   </si>
   <si>
@@ -54,24 +48,15 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>TonyQA</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
     <t>can't be blank</t>
   </si>
   <si>
-    <t>can be Male or Female</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
-    <t>can be Active or Inactive</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -94,6 +79,57 @@
   </si>
   <si>
     <t>Admin4@ukr.net</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
+    <t>Admin2</t>
+  </si>
+  <si>
+    <t>Admin3</t>
+  </si>
+  <si>
+    <t>Admin4</t>
+  </si>
+  <si>
+    <t>Admin7</t>
+  </si>
+  <si>
+    <t>Admin8</t>
+  </si>
+  <si>
+    <t>Admin9</t>
+  </si>
+  <si>
+    <t>Admin10</t>
+  </si>
+  <si>
+    <t>Admin11</t>
+  </si>
+  <si>
+    <t>Admin12</t>
+  </si>
+  <si>
+    <t>Admin13</t>
+  </si>
+  <si>
+    <t>Admin14</t>
+  </si>
+  <si>
+    <t>Admin15</t>
+  </si>
+  <si>
+    <t>Admin17</t>
+  </si>
+  <si>
+    <t>Admin19</t>
+  </si>
+  <si>
+    <t>Admin20</t>
+  </si>
+  <si>
+    <t>Admin21</t>
   </si>
 </sst>
 </file>
@@ -424,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,415 +475,343 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>-1</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>-1</v>
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>-1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>-1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="D15" r:id="rId2"/>
-    <hyperlink ref="B13" r:id="rId3"/>
-    <hyperlink ref="C14" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5" display="Admin3@ukr.net"/>
-    <hyperlink ref="B10" r:id="rId6" display="Admin2@ukr.net"/>
-    <hyperlink ref="B11" r:id="rId7" display="Admin2@ukr.net"/>
-    <hyperlink ref="B12" r:id="rId8" display="Admin2@ukr.net"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B15" r:id="rId10" display="Admin2@ukr.net"/>
-    <hyperlink ref="B16" r:id="rId11" display="Admin2@ukr.net"/>
-    <hyperlink ref="B17" r:id="rId12" display="Admin2@ukr.net"/>
-    <hyperlink ref="B18" r:id="rId13" display="Admin2@ukr.net"/>
-    <hyperlink ref="B19" r:id="rId14" display="Admin2@ukr.net"/>
-    <hyperlink ref="B20" r:id="rId15" display="Admin2@ukr.net"/>
-    <hyperlink ref="B21" r:id="rId16" display="Admin2@ukr.net"/>
-    <hyperlink ref="B7" r:id="rId17" display="Admin2@ukr.net"/>
-    <hyperlink ref="B5" r:id="rId18" display="Admin2@ukr.net"/>
-    <hyperlink ref="B3" r:id="rId19" display="Admin2@ukr.net"/>
-    <hyperlink ref="B22" r:id="rId20" display="!@#$%^"/>
-    <hyperlink ref="B23" r:id="rId21" display="!@#$%^"/>
+    <hyperlink ref="D13" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5" display="Admin2@ukr.net"/>
+    <hyperlink ref="B9" r:id="rId6" display="Admin2@ukr.net"/>
+    <hyperlink ref="B10" r:id="rId7" display="Admin2@ukr.net"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B13" r:id="rId9" display="Admin2@ukr.net"/>
+    <hyperlink ref="B14" r:id="rId10" display="Admin2@ukr.net"/>
+    <hyperlink ref="B15" r:id="rId11" display="Admin2@ukr.net"/>
+    <hyperlink ref="B16" r:id="rId12" display="Admin2@ukr.net"/>
+    <hyperlink ref="B17" r:id="rId13" display="Admin2@ukr.net"/>
+    <hyperlink ref="B5" r:id="rId14" display="Admin2@ukr.net"/>
+    <hyperlink ref="B3" r:id="rId15" display="Admin2@ukr.net"/>
+    <hyperlink ref="B18" r:id="rId16" display="!@#$%^"/>
+    <hyperlink ref="B19" r:id="rId17" display="!@#$%^"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>